<commit_message>
Worked on TC06 - Job Categories feature
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Add New Account" sheetId="1" r:id="rId1"/>
-    <sheet name="Add Job Title" sheetId="2" r:id="rId2"/>
+    <sheet name="01 - Add New Account" sheetId="1" r:id="rId1"/>
+    <sheet name="02 - Add Job Title" sheetId="2" r:id="rId2"/>
+    <sheet name="04 - Add Job Category" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>employeeName</t>
   </si>
@@ -99,6 +100,24 @@
   </si>
   <si>
     <t>Pembantu</t>
+  </si>
+  <si>
+    <t>jobCategoryName</t>
+  </si>
+  <si>
+    <t>IT Professional</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Health care</t>
+  </si>
+  <si>
+    <t>Painter</t>
+  </si>
+  <si>
+    <t>Barber</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1217,7 @@
   <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -1275,4 +1294,51 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on TC07 - Employee List feature
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="01 - Add New Account" sheetId="1" r:id="rId1"/>
     <sheet name="02 - Add Job Title" sheetId="2" r:id="rId2"/>
     <sheet name="04 - Add Job Category" sheetId="3" r:id="rId3"/>
+    <sheet name="05 - Add Employee" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>employeeName</t>
   </si>
@@ -118,6 +119,60 @@
   </si>
   <si>
     <t>Barber</t>
+  </si>
+  <si>
+    <t>empFirstName</t>
+  </si>
+  <si>
+    <t>empMidName</t>
+  </si>
+  <si>
+    <t>empLastName</t>
+  </si>
+  <si>
+    <t>empID</t>
+  </si>
+  <si>
+    <t>empUsername</t>
+  </si>
+  <si>
+    <t>empPassword</t>
+  </si>
+  <si>
+    <t>empPasswordConfirmaton</t>
+  </si>
+  <si>
+    <t>Ahmad</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>0299</t>
+  </si>
+  <si>
+    <t>ahmad098</t>
+  </si>
+  <si>
+    <t>jq6leojyGnb59OuxS61Hr0q+yqPfNELT</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Hasnul\\Katalon Studio\\Katalon-Studio-Training-Assessment\\OrangeHRM_Nafis\\File Upload Test Data\\19263862.png</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>Froberg</t>
+  </si>
+  <si>
+    <t>rickforob166</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Hasnul\\Katalon Studio\\Katalon-Studio-Training-Assessment\\OrangeHRM_Nafis\\File Upload Test Data\\43392873.png</t>
   </si>
 </sst>
 </file>
@@ -731,8 +786,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1301,7 +1360,7 @@
   <sheetPr/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -1341,4 +1400,117 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="15.2857142857143" customWidth="1"/>
+    <col min="2" max="3" width="14.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="7.42857142857143" customWidth="1"/>
+    <col min="5" max="5" width="15.1428571428571" customWidth="1"/>
+    <col min="6" max="7" width="29.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="6.85714285714286" customWidth="1"/>
+    <col min="9" max="9" width="131.285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>322</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <ignoredErrors>
+    <ignoredError sqref="D2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on TC07 - Employee List feature, 02 - Search Employee and edit 01 - Add Employee Test Data Excel
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="01 - Add New Account" sheetId="1" r:id="rId1"/>
     <sheet name="02 - Add Job Title" sheetId="2" r:id="rId2"/>
     <sheet name="04 - Add Job Category" sheetId="3" r:id="rId3"/>
-    <sheet name="05 - Add Employee" sheetId="4" r:id="rId4"/>
+    <sheet name="05 - Add Employee" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>employeeName</t>
   </si>
@@ -169,10 +169,40 @@
     <t>Froberg</t>
   </si>
   <si>
+    <t>0322</t>
+  </si>
+  <si>
     <t>rickforob166</t>
   </si>
   <si>
     <t>C:\\Users\\Hasnul\\Katalon Studio\\Katalon-Studio-Training-Assessment\\OrangeHRM_Nafis\\File Upload Test Data\\43392873.png</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Bok Bok</t>
+  </si>
+  <si>
+    <t>0666</t>
+  </si>
+  <si>
+    <t>alfredbok2</t>
+  </si>
+  <si>
+    <t>Zack</t>
+  </si>
+  <si>
+    <t>Junaidi</t>
+  </si>
+  <si>
+    <t>Apron</t>
+  </si>
+  <si>
+    <t>1066</t>
+  </si>
+  <si>
+    <t>zackapron99</t>
   </si>
 </sst>
 </file>
@@ -1405,22 +1435,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
-  <cols>
-    <col min="1" max="1" width="15.2857142857143" customWidth="1"/>
-    <col min="2" max="3" width="14.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="7.42857142857143" customWidth="1"/>
-    <col min="5" max="5" width="15.1428571428571" customWidth="1"/>
-    <col min="6" max="7" width="29.4285714285714" customWidth="1"/>
-    <col min="8" max="8" width="6.85714285714286" customWidth="1"/>
-    <col min="9" max="9" width="131.285714285714" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -1487,11 +1508,11 @@
       <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="D3">
-        <v>322</v>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
@@ -1503,14 +1524,63 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="D2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on TC05 - Add Pay Grade feature - Finished up 03 - Delete Currency test cases, edit 02 - Add Currency, and rename Test Data files
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="01 - Add New Account" sheetId="1" r:id="rId1"/>
-    <sheet name="02 - Add Job Title" sheetId="2" r:id="rId2"/>
-    <sheet name="04 - Add Job Category" sheetId="3" r:id="rId3"/>
-    <sheet name="05 - Add Employee" sheetId="5" r:id="rId4"/>
+    <sheet name="TC03-02 Add New Account" sheetId="1" r:id="rId1"/>
+    <sheet name="TC04-01 Add Job Title" sheetId="2" r:id="rId2"/>
+    <sheet name="TC05-01 Add New Currency" sheetId="7" r:id="rId3"/>
+    <sheet name="TC05-03 Delete Currencies" sheetId="6" r:id="rId4"/>
+    <sheet name="TC06-01 Add Job Category" sheetId="3" r:id="rId5"/>
+    <sheet name="TC07-01 - Add Employee" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>employeeName</t>
   </si>
@@ -101,6 +103,48 @@
   </si>
   <si>
     <t>Pembantu</t>
+  </si>
+  <si>
+    <t>payGradeName</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>minimumSalary</t>
+  </si>
+  <si>
+    <t>maximumSalary</t>
+  </si>
+  <si>
+    <t>EUR - Euro</t>
+  </si>
+  <si>
+    <t>FJD - Fiji Dollar</t>
+  </si>
+  <si>
+    <t>AED - Utd. Arab Emir. Dirham</t>
+  </si>
+  <si>
+    <t>ALL - Albanian Lek</t>
+  </si>
+  <si>
+    <t>XAU - Gold (oz.)</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>Fiji Dollar</t>
+  </si>
+  <si>
+    <t>Utd. Arab Emir. Dirham</t>
+  </si>
+  <si>
+    <t>Albanian Lek</t>
+  </si>
+  <si>
+    <t>Gold (oz.)</t>
   </si>
   <si>
     <t>jobCategoryName</t>
@@ -816,10 +860,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
@@ -1388,6 +1435,109 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F11:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" ht="30" spans="2:2">
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1398,32 +1548,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1432,38 +1582,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1474,106 +1624,106 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H5">
         <v>2</v>

</xml_diff>

<commit_message>
Worked on TC03 Users feature, touched up 03 - Delete Account Test Cases
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" firstSheet="2" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="TC03-02 Add New Account" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>employeeName</t>
   </si>
@@ -54,6 +54,12 @@
     <t>janeander444</t>
   </si>
   <si>
+    <t>Nathan  Elliot</t>
+  </si>
+  <si>
+    <t>PeterWah2</t>
+  </si>
+  <si>
     <t>Peter Mac Anderson</t>
   </si>
   <si>
@@ -64,6 +70,12 @@
   </si>
   <si>
     <t>teracso098</t>
+  </si>
+  <si>
+    <t>Charlie  Carter</t>
+  </si>
+  <si>
+    <t>thihan7</t>
   </si>
   <si>
     <t>jobTitle</t>
@@ -1188,13 +1200,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="17.5714285714286" customWidth="1"/>
@@ -1296,18 +1308,18 @@
         <v>8</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1319,15 +1331,15 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1336,10 +1348,50 @@
         <v>8</v>
       </c>
       <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
-      <c r="F7">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1364,66 +1416,66 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1437,7 +1489,7 @@
   <sheetPr/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
@@ -1445,41 +1497,41 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" ht="30" spans="2:2">
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1501,32 +1553,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1548,32 +1600,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1595,135 +1647,135 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H5">
         <v>2</v>

</xml_diff>

<commit_message>
Worked on TC07 - Employee List feature, touched up 03 - Delete Employee Record Test Cases
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650"/>
+    <workbookView windowWidth="20490" windowHeight="7650" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TC03-02 Add New Account" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>employeeName</t>
   </si>
@@ -198,7 +198,7 @@
     <t>empPasswordConfirmaton</t>
   </si>
   <si>
-    <t>Ahmad</t>
+    <t>Ahmadi</t>
   </si>
   <si>
     <t>Tim</t>
@@ -207,7 +207,7 @@
     <t>Sean</t>
   </si>
   <si>
-    <t>0299</t>
+    <t>0661</t>
   </si>
   <si>
     <t>ahmad098</t>
@@ -219,13 +219,61 @@
     <t>C:\\Users\\Hasnul\\Katalon Studio\\Katalon-Studio-Training-Assessment\\OrangeHRM_Nafis\\File Upload Test Data\\19263862.png</t>
   </si>
   <si>
+    <t>Berryl</t>
+  </si>
+  <si>
+    <t>Chow</t>
+  </si>
+  <si>
+    <t>0662</t>
+  </si>
+  <si>
+    <t>berry121</t>
+  </si>
+  <si>
+    <t>Drews</t>
+  </si>
+  <si>
+    <t>Berry</t>
+  </si>
+  <si>
+    <t>0663</t>
+  </si>
+  <si>
+    <t>dre21</t>
+  </si>
+  <si>
+    <t>Eriksen</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>0664</t>
+  </si>
+  <si>
+    <t>eridave33</t>
+  </si>
+  <si>
+    <t>Alley</t>
+  </si>
+  <si>
+    <t>Way</t>
+  </si>
+  <si>
+    <t>0665</t>
+  </si>
+  <si>
+    <t>alley12</t>
+  </si>
+  <si>
     <t>Rick</t>
   </si>
   <si>
     <t>Froberg</t>
   </si>
   <si>
-    <t>0322</t>
+    <t>0666</t>
   </si>
   <si>
     <t>rickforob166</t>
@@ -238,9 +286,6 @@
   </si>
   <si>
     <t>Bok Bok</t>
-  </si>
-  <si>
-    <t>0666</t>
   </si>
   <si>
     <t>alfredbok2</t>
@@ -872,10 +917,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1202,7 +1250,7 @@
   <sheetPr/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1515,7 +1563,7 @@
       </c>
     </row>
     <row r="3" ht="30" spans="2:2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1562,7 +1610,7 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1637,13 +1685,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -1684,7 +1732,7 @@
       <c r="C2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E2" t="s">
@@ -1703,14 +1751,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E3" t="s">
@@ -1723,24 +1771,21 @@
         <v>64</v>
       </c>
       <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" t="s">
-        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>64</v>
@@ -1748,28 +1793,22 @@
       <c r="G4" t="s">
         <v>64</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
+      <c r="H4" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>77</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
       </c>
       <c r="F5" t="s">
         <v>64</v>
@@ -1777,7 +1816,108 @@
       <c r="G5" t="s">
         <v>64</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Worked on TC05 - Pay Grades feature, Add more BDD to 02 - Add Currenct and 03 - Delete Currency
</commit_message>
<xml_diff>
--- a/OrangeHRM_Nafis/Data Files/Test Data.xlsx
+++ b/OrangeHRM_Nafis/Data Files/Test Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" firstSheet="3" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7650" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TC03-02 Add New Account" sheetId="1" r:id="rId1"/>
@@ -1538,7 +1538,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F11:F12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
@@ -1593,7 +1593,7 @@
   <sheetPr/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
@@ -1687,7 +1687,7 @@
   <sheetPr/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>